<commit_message>
Commit EL paper doc
</commit_message>
<xml_diff>
--- a/AuthorList.xlsx
+++ b/AuthorList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sorel/next/next-exp/NEXTAuthorList/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mistryk2/OneDrive - University of Texas at Arlington/Code/NEXTAuthorList/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30A2D67F-286E-CC41-BEF0-2428FE27E9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44BDB05C-0641-B847-9E3F-73667200CD89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="2240" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AuthorList" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="478" uniqueCount="248">
   <si>
     <t>LastName</t>
   </si>
@@ -734,13 +734,43 @@
   </si>
   <si>
     <t>Seemann</t>
+  </si>
+  <si>
+    <t>Oliver</t>
+  </si>
+  <si>
+    <t>D.</t>
+  </si>
+  <si>
+    <t>University of Texas at El Paso</t>
+  </si>
+  <si>
+    <t>500 W. University Ave., El Paso, Texas 79968, USA.</t>
+  </si>
+  <si>
+    <t>Munson</t>
+  </si>
+  <si>
+    <t>Norman</t>
+  </si>
+  <si>
+    <t>Pingulkar</t>
+  </si>
+  <si>
+    <t>Rodriguez-Tiscareno</t>
+  </si>
+  <si>
+    <t>Silva</t>
+  </si>
+  <si>
+    <t>Stogsdill</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -871,6 +901,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1217,8 +1254,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1574,13 +1612,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H107"/>
+  <dimension ref="A1:H114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A94" sqref="A94"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="5" max="5" width="98.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -2379,6 +2420,9 @@
       <c r="B54" t="s">
         <v>211</v>
       </c>
+      <c r="D54">
+        <v>3</v>
+      </c>
       <c r="E54" t="s">
         <v>58</v>
       </c>
@@ -2575,6 +2619,9 @@
       <c r="B68" t="s">
         <v>143</v>
       </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
       <c r="E68" t="s">
         <v>58</v>
       </c>
@@ -2716,221 +2763,227 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>155</v>
+        <v>238</v>
       </c>
       <c r="B78" t="s">
-        <v>145</v>
+        <v>239</v>
+      </c>
+      <c r="D78">
+        <v>6</v>
       </c>
       <c r="E78" t="s">
-        <v>48</v>
+        <v>240</v>
       </c>
       <c r="F78" t="s">
-        <v>49</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B79" t="s">
-        <v>224</v>
+        <v>145</v>
       </c>
       <c r="E79" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="F79" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B80" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="E80" t="s">
-        <v>127</v>
+        <v>14</v>
       </c>
       <c r="F80" t="s">
-        <v>128</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B81" t="s">
-        <v>159</v>
+        <v>225</v>
       </c>
       <c r="E81" t="s">
-        <v>58</v>
+        <v>127</v>
       </c>
       <c r="F81" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B82" t="s">
-        <v>145</v>
+        <v>159</v>
       </c>
       <c r="E82" t="s">
-        <v>45</v>
+        <v>58</v>
       </c>
       <c r="F82" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B83" t="s">
-        <v>44</v>
+        <v>145</v>
       </c>
       <c r="E83" t="s">
-        <v>79</v>
+        <v>45</v>
       </c>
       <c r="F83" t="s">
-        <v>115</v>
+        <v>22</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B84" t="s">
-        <v>217</v>
+        <v>44</v>
       </c>
       <c r="E84" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="F84" t="s">
-        <v>62</v>
+        <v>115</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B85" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="E85" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="F85" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B86" t="s">
-        <v>215</v>
+        <v>226</v>
       </c>
       <c r="E86" t="s">
-        <v>79</v>
+        <v>27</v>
       </c>
       <c r="F86" t="s">
-        <v>80</v>
+        <v>28</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B87" t="s">
-        <v>159</v>
+        <v>215</v>
       </c>
       <c r="E87" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="F87" t="s">
-        <v>22</v>
-      </c>
-      <c r="G87" t="s">
-        <v>92</v>
-      </c>
-      <c r="H87" t="s">
-        <v>93</v>
+        <v>80</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B88" t="s">
-        <v>9</v>
+        <v>159</v>
       </c>
       <c r="E88" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F88" t="s">
         <v>22</v>
       </c>
+      <c r="G88" t="s">
+        <v>92</v>
+      </c>
+      <c r="H88" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B89" t="s">
-        <v>212</v>
+        <v>9</v>
       </c>
       <c r="E89" t="s">
-        <v>10</v>
+        <v>56</v>
       </c>
       <c r="F89" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B90" t="s">
-        <v>224</v>
+        <v>212</v>
+      </c>
+      <c r="D90">
+        <v>2</v>
       </c>
       <c r="E90" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="F90" t="s">
-        <v>22</v>
-      </c>
-      <c r="H90" t="s">
-        <v>49</v>
+        <v>11</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B91" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="E91" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F91" t="s">
-        <v>62</v>
+        <v>22</v>
+      </c>
+      <c r="H91" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B92" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E92" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="F92" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -2938,10 +2991,10 @@
         <v>170</v>
       </c>
       <c r="B93" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E93" t="s">
-        <v>90</v>
+        <v>53</v>
       </c>
       <c r="F93" t="s">
         <v>70</v>
@@ -2949,52 +3002,52 @@
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
-        <v>237</v>
+        <v>170</v>
       </c>
       <c r="B94" t="s">
-        <v>44</v>
+        <v>229</v>
       </c>
       <c r="E94" t="s">
-        <v>45</v>
+        <v>90</v>
       </c>
       <c r="F94" t="s">
-        <v>22</v>
+        <v>70</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
-        <v>171</v>
+        <v>237</v>
       </c>
       <c r="B95" t="s">
-        <v>159</v>
+        <v>44</v>
       </c>
       <c r="E95" t="s">
-        <v>117</v>
+        <v>45</v>
       </c>
       <c r="F95" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B96" t="s">
-        <v>230</v>
+        <v>159</v>
       </c>
       <c r="E96" t="s">
-        <v>45</v>
+        <v>117</v>
       </c>
       <c r="F96" t="s">
-        <v>22</v>
+        <v>118</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B97" t="s">
-        <v>174</v>
+        <v>230</v>
       </c>
       <c r="E97" t="s">
         <v>45</v>
@@ -3005,24 +3058,24 @@
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="B98" t="s">
-        <v>217</v>
+        <v>174</v>
       </c>
       <c r="E98" t="s">
-        <v>61</v>
+        <v>45</v>
       </c>
       <c r="F98" t="s">
-        <v>62</v>
+        <v>22</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B99" t="s">
-        <v>145</v>
+        <v>217</v>
       </c>
       <c r="E99" t="s">
         <v>61</v>
@@ -3033,120 +3086,234 @@
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B100" t="s">
-        <v>178</v>
+        <v>145</v>
       </c>
       <c r="E100" t="s">
-        <v>90</v>
+        <v>61</v>
       </c>
       <c r="F100" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="B101" t="s">
-        <v>231</v>
+        <v>178</v>
       </c>
       <c r="E101" t="s">
-        <v>17</v>
+        <v>90</v>
       </c>
       <c r="F101" t="s">
-        <v>18</v>
+        <v>70</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B102" t="s">
-        <v>215</v>
+        <v>231</v>
       </c>
       <c r="E102" t="s">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="F102" t="s">
-        <v>22</v>
-      </c>
-      <c r="G102" t="s">
-        <v>181</v>
-      </c>
-      <c r="H102" t="s">
-        <v>182</v>
+        <v>18</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="B103" t="s">
-        <v>47</v>
+        <v>215</v>
       </c>
       <c r="E103" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
       <c r="F103" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+      <c r="G103" t="s">
+        <v>181</v>
+      </c>
+      <c r="H103" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B104" t="s">
-        <v>225</v>
+        <v>47</v>
       </c>
       <c r="E104" t="s">
-        <v>61</v>
+        <v>14</v>
       </c>
       <c r="F104" t="s">
-        <v>62</v>
+        <v>15</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B105" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="E105" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="F105" t="s">
-        <v>95</v>
+        <v>62</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B106" t="s">
-        <v>187</v>
+        <v>232</v>
       </c>
       <c r="E106" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="F106" t="s">
-        <v>15</v>
+        <v>95</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>186</v>
+      </c>
+      <c r="B107" t="s">
+        <v>187</v>
+      </c>
+      <c r="E107" t="s">
+        <v>14</v>
+      </c>
+      <c r="F107" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
         <v>235</v>
       </c>
-      <c r="B107" t="s">
+      <c r="B108" t="s">
         <v>47</v>
       </c>
-      <c r="E107" t="s">
+      <c r="E108" t="s">
         <v>45</v>
       </c>
-      <c r="F107" t="s">
+      <c r="F108" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>242</v>
+      </c>
+      <c r="B109" t="s">
+        <v>20</v>
+      </c>
+      <c r="D109">
+        <v>4</v>
+      </c>
+      <c r="E109" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F109" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G109" s="1"/>
+    </row>
+    <row r="110" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>243</v>
+      </c>
+      <c r="B110" t="s">
+        <v>68</v>
+      </c>
+      <c r="D110">
+        <v>5</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F110" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>244</v>
+      </c>
+      <c r="B111" t="s">
+        <v>35</v>
+      </c>
+      <c r="D111">
+        <v>7</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F111" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>245</v>
+      </c>
+      <c r="B112" t="s">
+        <v>44</v>
+      </c>
+      <c r="D112">
+        <v>8</v>
+      </c>
+      <c r="E112" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F112" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>246</v>
+      </c>
+      <c r="B113" t="s">
+        <v>143</v>
+      </c>
+      <c r="D113">
+        <v>9</v>
+      </c>
+      <c r="E113" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>247</v>
+      </c>
+      <c r="B114" t="s">
+        <v>143</v>
+      </c>
+      <c r="D114">
+        <v>10</v>
+      </c>
+      <c r="E114" s="1" t="s">
+        <v>58</v>
       </c>
     </row>
   </sheetData>

</xml_diff>